<commit_message>
Added logo and changed app display name
</commit_message>
<xml_diff>
--- a/ArcDataCollection.xlsx
+++ b/ArcDataCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaseking/AndroidStudioProjects/CS3560AppGit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E401A6A3-D661-2D4D-8A21-D81D9E2BE7B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CE7EA7-0127-A94D-84C6-3E2124A76E9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,15 @@
     <sheet name="Monday 9-23-19" sheetId="7" r:id="rId7"/>
     <sheet name="Tuesday 9-24-19" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -415,6 +423,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -434,13 +443,12 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,18 +692,18 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -703,10 +711,10 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -739,7 +747,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -757,7 +765,7 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -765,7 +773,7 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -773,7 +781,7 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -781,7 +789,7 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
@@ -789,7 +797,7 @@
       <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -797,7 +805,7 @@
       <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -805,7 +813,7 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -813,7 +821,7 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -821,7 +829,7 @@
       <c r="L12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -837,10 +845,10 @@
       <c r="L13" s="17"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="19">
         <v>214</v>
       </c>
@@ -856,16 +864,16 @@
       <c r="G16" s="19">
         <v>227</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -876,7 +884,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="10"/>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -885,103 +893,103 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="I18" s="34"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="I20" s="34"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="I21" s="34"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="I22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="12"/>
-      <c r="I23" s="34"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="I24" s="34"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="I25" s="34"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -990,7 +998,7 @@
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="17"/>
-      <c r="I26" s="35"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1017,8 +1025,8 @@
   </sheetPr>
   <dimension ref="A1:Q192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E176" sqref="E176"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1040,18 +1048,18 @@
     <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -1059,10 +1067,10 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1103,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1113,7 +1121,7 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1121,7 +1129,7 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1129,7 +1137,7 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1137,7 +1145,7 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1145,7 +1153,7 @@
       <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1161,7 @@
       <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1161,7 +1169,7 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1177,7 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1177,7 +1185,7 @@
       <c r="L12" s="12"/>
     </row>
     <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1213,10 +1221,10 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="19">
         <v>214</v>
       </c>
@@ -1232,16 +1240,16 @@
       <c r="G16" s="19">
         <v>227</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1252,7 +1260,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="10"/>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -1261,103 +1269,103 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="I18" s="34"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="I20" s="34"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="I21" s="34"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="I22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="12"/>
-      <c r="I23" s="34"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="I24" s="34"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="I25" s="34"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1376,7 +1384,7 @@
       <c r="G26" s="18">
         <v>1</v>
       </c>
-      <c r="I26" s="35"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1385,10 +1393,10 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="7" t="s">
         <v>4</v>
       </c>
@@ -1421,7 +1429,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1439,7 +1447,7 @@
       <c r="L30" s="10"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="5" t="s">
         <v>8</v>
       </c>
@@ -1447,7 +1455,7 @@
       <c r="L31" s="12"/>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="5" t="s">
         <v>9</v>
       </c>
@@ -1455,7 +1463,7 @@
       <c r="L32" s="12"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="5" t="s">
         <v>10</v>
       </c>
@@ -1463,7 +1471,7 @@
       <c r="L33" s="12"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="34"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="5" t="s">
         <v>11</v>
       </c>
@@ -1471,7 +1479,7 @@
       <c r="L34" s="12"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="5" t="s">
         <v>12</v>
       </c>
@@ -1479,7 +1487,7 @@
       <c r="L35" s="12"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="5" t="s">
         <v>13</v>
       </c>
@@ -1487,7 +1495,7 @@
       <c r="L36" s="12"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="5" t="s">
         <v>14</v>
       </c>
@@ -1495,7 +1503,7 @@
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="34"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="5" t="s">
         <v>15</v>
       </c>
@@ -1503,7 +1511,7 @@
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="35"/>
+      <c r="A39" s="36"/>
       <c r="B39" s="5" t="s">
         <v>16</v>
       </c>
@@ -1546,19 +1554,19 @@
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="37"/>
-      <c r="L41" s="38"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="39"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B42" s="43"/>
@@ -1577,16 +1585,16 @@
       <c r="G42" s="19">
         <v>227</v>
       </c>
-      <c r="I42" s="41" t="s">
+      <c r="I42" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="42"/>
+      <c r="J42" s="44"/>
       <c r="K42" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -1597,7 +1605,7 @@
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="10"/>
-      <c r="I43" s="33" t="s">
+      <c r="I43" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J43" s="5" t="s">
@@ -1606,103 +1614,103 @@
       <c r="K43" s="10"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G44" s="12"/>
-      <c r="I44" s="34"/>
+      <c r="I44" s="35"/>
       <c r="J44" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K44" s="12"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="34"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="12"/>
-      <c r="I45" s="34"/>
+      <c r="I45" s="35"/>
       <c r="J45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K45" s="12"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="34"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="12"/>
-      <c r="I46" s="34"/>
+      <c r="I46" s="35"/>
       <c r="J46" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K46" s="12"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="34"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G47" s="12"/>
-      <c r="I47" s="34"/>
+      <c r="I47" s="35"/>
       <c r="J47" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K47" s="12"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="34"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G48" s="12"/>
-      <c r="I48" s="34"/>
+      <c r="I48" s="35"/>
       <c r="J48" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K48" s="12"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="12"/>
-      <c r="I49" s="34"/>
+      <c r="I49" s="35"/>
       <c r="J49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K49" s="12"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="34"/>
+      <c r="A50" s="35"/>
       <c r="B50" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G50" s="12"/>
-      <c r="I50" s="34"/>
+      <c r="I50" s="35"/>
       <c r="J50" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K50" s="12"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="34"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G51" s="12"/>
-      <c r="I51" s="34"/>
+      <c r="I51" s="35"/>
       <c r="J51" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K51" s="12"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="35"/>
+      <c r="A52" s="36"/>
       <c r="B52" s="5" t="s">
         <v>16</v>
       </c>
@@ -1721,7 +1729,7 @@
       <c r="G52" s="26">
         <v>1</v>
       </c>
-      <c r="I52" s="35"/>
+      <c r="I52" s="36"/>
       <c r="J52" s="5" t="s">
         <v>16</v>
       </c>
@@ -1741,24 +1749,24 @@
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="36" t="s">
+      <c r="C56" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
-      <c r="L56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
+      <c r="L56" s="39"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="38"/>
+      <c r="B57" s="39"/>
       <c r="C57" s="7" t="s">
         <v>4</v>
       </c>
@@ -1791,7 +1799,7 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -1809,7 +1817,7 @@
       <c r="L58" s="10"/>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="34"/>
+      <c r="A59" s="35"/>
       <c r="B59" s="5" t="s">
         <v>8</v>
       </c>
@@ -1817,7 +1825,7 @@
       <c r="L59" s="12"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="34"/>
+      <c r="A60" s="35"/>
       <c r="B60" s="5" t="s">
         <v>9</v>
       </c>
@@ -1825,7 +1833,7 @@
       <c r="L60" s="12"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="34"/>
+      <c r="A61" s="35"/>
       <c r="B61" s="5" t="s">
         <v>10</v>
       </c>
@@ -1833,7 +1841,7 @@
       <c r="L61" s="12"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="34"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="5" t="s">
         <v>11</v>
       </c>
@@ -1841,7 +1849,7 @@
       <c r="L62" s="12"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="34"/>
+      <c r="A63" s="35"/>
       <c r="B63" s="5" t="s">
         <v>12</v>
       </c>
@@ -1849,7 +1857,7 @@
       <c r="L63" s="12"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="34"/>
+      <c r="A64" s="35"/>
       <c r="B64" s="5" t="s">
         <v>13</v>
       </c>
@@ -1857,7 +1865,7 @@
       <c r="L64" s="12"/>
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="34"/>
+      <c r="A65" s="35"/>
       <c r="B65" s="5" t="s">
         <v>14</v>
       </c>
@@ -1865,7 +1873,7 @@
       <c r="L65" s="12"/>
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="34"/>
+      <c r="A66" s="35"/>
       <c r="B66" s="5" t="s">
         <v>15</v>
       </c>
@@ -1901,7 +1909,7 @@
       </c>
     </row>
     <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="35"/>
+      <c r="A67" s="36"/>
       <c r="B67" s="5" t="s">
         <v>16</v>
       </c>
@@ -1917,10 +1925,10 @@
       <c r="L67" s="17"/>
     </row>
     <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="40" t="s">
+      <c r="A70" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B70" s="38"/>
+      <c r="B70" s="39"/>
       <c r="C70" s="19">
         <v>214</v>
       </c>
@@ -1936,16 +1944,16 @@
       <c r="G70" s="19">
         <v>227</v>
       </c>
-      <c r="I70" s="41" t="s">
+      <c r="I70" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J70" s="38"/>
+      <c r="J70" s="39"/>
       <c r="K70" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -1956,7 +1964,7 @@
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="10"/>
-      <c r="I71" s="33" t="s">
+      <c r="I71" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J71" s="5" t="s">
@@ -1965,91 +1973,91 @@
       <c r="K71" s="10"/>
     </row>
     <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="34"/>
+      <c r="A72" s="35"/>
       <c r="B72" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G72" s="12"/>
-      <c r="I72" s="34"/>
+      <c r="I72" s="35"/>
       <c r="J72" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K72" s="12"/>
     </row>
     <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="34"/>
+      <c r="A73" s="35"/>
       <c r="B73" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G73" s="12"/>
-      <c r="I73" s="34"/>
+      <c r="I73" s="35"/>
       <c r="J73" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K73" s="12"/>
     </row>
     <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="34"/>
+      <c r="A74" s="35"/>
       <c r="B74" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G74" s="12"/>
-      <c r="I74" s="34"/>
+      <c r="I74" s="35"/>
       <c r="J74" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K74" s="12"/>
     </row>
     <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="34"/>
+      <c r="A75" s="35"/>
       <c r="B75" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G75" s="12"/>
-      <c r="I75" s="34"/>
+      <c r="I75" s="35"/>
       <c r="J75" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K75" s="12"/>
     </row>
     <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="34"/>
+      <c r="A76" s="35"/>
       <c r="B76" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G76" s="12"/>
-      <c r="I76" s="34"/>
+      <c r="I76" s="35"/>
       <c r="J76" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K76" s="12"/>
     </row>
     <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="34"/>
+      <c r="A77" s="35"/>
       <c r="B77" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="12"/>
-      <c r="I77" s="34"/>
+      <c r="I77" s="35"/>
       <c r="J77" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K77" s="12"/>
     </row>
     <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="34"/>
+      <c r="A78" s="35"/>
       <c r="B78" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G78" s="12"/>
-      <c r="I78" s="34"/>
+      <c r="I78" s="35"/>
       <c r="J78" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K78" s="12"/>
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="34"/>
+      <c r="A79" s="35"/>
       <c r="B79" s="5" t="s">
         <v>15</v>
       </c>
@@ -2068,7 +2076,7 @@
       <c r="G79" s="27">
         <v>1</v>
       </c>
-      <c r="I79" s="34"/>
+      <c r="I79" s="35"/>
       <c r="J79" s="5" t="s">
         <v>15</v>
       </c>
@@ -2077,7 +2085,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="35"/>
+      <c r="A80" s="36"/>
       <c r="B80" s="5" t="s">
         <v>16</v>
       </c>
@@ -2086,7 +2094,7 @@
       <c r="E80" s="15"/>
       <c r="F80" s="15"/>
       <c r="G80" s="17"/>
-      <c r="I80" s="35"/>
+      <c r="I80" s="36"/>
       <c r="J80" s="5" t="s">
         <v>16</v>
       </c>
@@ -2106,24 +2114,24 @@
     <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
-      <c r="C84" s="36" t="s">
+      <c r="C84" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="37"/>
-      <c r="H84" s="37"/>
-      <c r="I84" s="37"/>
-      <c r="J84" s="37"/>
-      <c r="K84" s="37"/>
-      <c r="L84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="38"/>
+      <c r="J84" s="38"/>
+      <c r="K84" s="38"/>
+      <c r="L84" s="39"/>
     </row>
     <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="39" t="s">
+      <c r="A85" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="38"/>
+      <c r="B85" s="39"/>
       <c r="C85" s="7" t="s">
         <v>4</v>
       </c>
@@ -2156,7 +2164,7 @@
       </c>
     </row>
     <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="33" t="s">
+      <c r="A86" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B86" s="5" t="s">
@@ -2174,7 +2182,7 @@
       <c r="L86" s="10"/>
     </row>
     <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="34"/>
+      <c r="A87" s="35"/>
       <c r="B87" s="5" t="s">
         <v>8</v>
       </c>
@@ -2182,7 +2190,7 @@
       <c r="L87" s="12"/>
     </row>
     <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="34"/>
+      <c r="A88" s="35"/>
       <c r="B88" s="5" t="s">
         <v>9</v>
       </c>
@@ -2190,7 +2198,7 @@
       <c r="L88" s="12"/>
     </row>
     <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="34"/>
+      <c r="A89" s="35"/>
       <c r="B89" s="5" t="s">
         <v>10</v>
       </c>
@@ -2198,7 +2206,7 @@
       <c r="L89" s="12"/>
     </row>
     <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="34"/>
+      <c r="A90" s="35"/>
       <c r="B90" s="5" t="s">
         <v>11</v>
       </c>
@@ -2206,7 +2214,7 @@
       <c r="L90" s="12"/>
     </row>
     <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="34"/>
+      <c r="A91" s="35"/>
       <c r="B91" s="5" t="s">
         <v>12</v>
       </c>
@@ -2214,7 +2222,7 @@
       <c r="L91" s="12"/>
     </row>
     <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="34"/>
+      <c r="A92" s="35"/>
       <c r="B92" s="5" t="s">
         <v>13</v>
       </c>
@@ -2250,7 +2258,7 @@
       </c>
     </row>
     <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="34"/>
+      <c r="A93" s="35"/>
       <c r="B93" s="5" t="s">
         <v>14</v>
       </c>
@@ -2286,7 +2294,7 @@
       </c>
     </row>
     <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="34"/>
+      <c r="A94" s="35"/>
       <c r="B94" s="5" t="s">
         <v>15</v>
       </c>
@@ -2294,7 +2302,7 @@
       <c r="L94" s="12"/>
     </row>
     <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="35"/>
+      <c r="A95" s="36"/>
       <c r="B95" s="5" t="s">
         <v>16</v>
       </c>
@@ -2310,10 +2318,10 @@
       <c r="L95" s="17"/>
     </row>
     <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="40" t="s">
+      <c r="A98" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B98" s="38"/>
+      <c r="B98" s="39"/>
       <c r="C98" s="19">
         <v>214</v>
       </c>
@@ -2329,16 +2337,16 @@
       <c r="G98" s="19">
         <v>227</v>
       </c>
-      <c r="I98" s="41" t="s">
+      <c r="I98" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J98" s="38"/>
+      <c r="J98" s="39"/>
       <c r="K98" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="33" t="s">
+      <c r="A99" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B99" s="5" t="s">
@@ -2349,7 +2357,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
       <c r="G99" s="10"/>
-      <c r="I99" s="33" t="s">
+      <c r="I99" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J99" s="5" t="s">
@@ -2358,67 +2366,67 @@
       <c r="K99" s="10"/>
     </row>
     <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="34"/>
+      <c r="A100" s="35"/>
       <c r="B100" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G100" s="12"/>
-      <c r="I100" s="34"/>
+      <c r="I100" s="35"/>
       <c r="J100" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K100" s="12"/>
     </row>
     <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="34"/>
+      <c r="A101" s="35"/>
       <c r="B101" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G101" s="12"/>
-      <c r="I101" s="34"/>
+      <c r="I101" s="35"/>
       <c r="J101" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K101" s="12"/>
     </row>
     <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="34"/>
+      <c r="A102" s="35"/>
       <c r="B102" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G102" s="12"/>
-      <c r="I102" s="34"/>
+      <c r="I102" s="35"/>
       <c r="J102" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K102" s="12"/>
     </row>
     <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="34"/>
+      <c r="A103" s="35"/>
       <c r="B103" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G103" s="12"/>
-      <c r="I103" s="34"/>
+      <c r="I103" s="35"/>
       <c r="J103" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K103" s="12"/>
     </row>
     <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="34"/>
+      <c r="A104" s="35"/>
       <c r="B104" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G104" s="12"/>
-      <c r="I104" s="34"/>
+      <c r="I104" s="35"/>
       <c r="J104" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K104" s="12"/>
     </row>
     <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="34"/>
+      <c r="A105" s="35"/>
       <c r="B105" s="5" t="s">
         <v>13</v>
       </c>
@@ -2437,7 +2445,7 @@
       <c r="G105" s="27">
         <v>1</v>
       </c>
-      <c r="I105" s="34"/>
+      <c r="I105" s="35"/>
       <c r="J105" s="5" t="s">
         <v>13</v>
       </c>
@@ -2446,7 +2454,7 @@
       </c>
     </row>
     <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="34"/>
+      <c r="A106" s="35"/>
       <c r="B106" s="5" t="s">
         <v>14</v>
       </c>
@@ -2465,7 +2473,7 @@
       <c r="G106" s="27">
         <v>1</v>
       </c>
-      <c r="I106" s="34"/>
+      <c r="I106" s="35"/>
       <c r="J106" s="5" t="s">
         <v>14</v>
       </c>
@@ -2474,19 +2482,19 @@
       </c>
     </row>
     <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="34"/>
+      <c r="A107" s="35"/>
       <c r="B107" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G107" s="12"/>
-      <c r="I107" s="34"/>
+      <c r="I107" s="35"/>
       <c r="J107" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K107" s="12"/>
     </row>
     <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="35"/>
+      <c r="A108" s="36"/>
       <c r="B108" s="5" t="s">
         <v>16</v>
       </c>
@@ -2495,7 +2503,7 @@
       <c r="E108" s="15"/>
       <c r="F108" s="15"/>
       <c r="G108" s="17"/>
-      <c r="I108" s="35"/>
+      <c r="I108" s="36"/>
       <c r="J108" s="5" t="s">
         <v>16</v>
       </c>
@@ -2513,24 +2521,24 @@
     <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
-      <c r="C112" s="36" t="s">
+      <c r="C112" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D112" s="37"/>
-      <c r="E112" s="37"/>
-      <c r="F112" s="37"/>
-      <c r="G112" s="37"/>
-      <c r="H112" s="37"/>
-      <c r="I112" s="37"/>
-      <c r="J112" s="37"/>
-      <c r="K112" s="37"/>
-      <c r="L112" s="38"/>
+      <c r="D112" s="38"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="38"/>
+      <c r="I112" s="38"/>
+      <c r="J112" s="38"/>
+      <c r="K112" s="38"/>
+      <c r="L112" s="39"/>
     </row>
     <row r="113" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="39" t="s">
+      <c r="A113" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B113" s="38"/>
+      <c r="B113" s="39"/>
       <c r="C113" s="7" t="s">
         <v>4</v>
       </c>
@@ -2563,7 +2571,7 @@
       </c>
     </row>
     <row r="114" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="33" t="s">
+      <c r="A114" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B114" s="5" t="s">
@@ -2581,7 +2589,7 @@
       <c r="L114" s="10"/>
     </row>
     <row r="115" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="34"/>
+      <c r="A115" s="35"/>
       <c r="B115" s="5" t="s">
         <v>8</v>
       </c>
@@ -2589,7 +2597,7 @@
       <c r="L115" s="12"/>
     </row>
     <row r="116" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="34"/>
+      <c r="A116" s="35"/>
       <c r="B116" s="5" t="s">
         <v>9</v>
       </c>
@@ -2597,7 +2605,7 @@
       <c r="L116" s="12"/>
     </row>
     <row r="117" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="34"/>
+      <c r="A117" s="35"/>
       <c r="B117" s="5" t="s">
         <v>10</v>
       </c>
@@ -2605,7 +2613,7 @@
       <c r="L117" s="12"/>
     </row>
     <row r="118" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="34"/>
+      <c r="A118" s="35"/>
       <c r="B118" s="5" t="s">
         <v>11</v>
       </c>
@@ -2613,7 +2621,7 @@
       <c r="L118" s="12"/>
     </row>
     <row r="119" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="34"/>
+      <c r="A119" s="35"/>
       <c r="B119" s="5" t="s">
         <v>12</v>
       </c>
@@ -2621,7 +2629,7 @@
       <c r="L119" s="12"/>
     </row>
     <row r="120" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="34"/>
+      <c r="A120" s="35"/>
       <c r="B120" s="5" t="s">
         <v>13</v>
       </c>
@@ -2629,7 +2637,7 @@
       <c r="L120" s="12"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="34"/>
+      <c r="A121" s="35"/>
       <c r="B121" s="5" t="s">
         <v>14</v>
       </c>
@@ -2637,7 +2645,7 @@
       <c r="L121" s="12"/>
     </row>
     <row r="122" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="34"/>
+      <c r="A122" s="35"/>
       <c r="B122" s="5" t="s">
         <v>15</v>
       </c>
@@ -2645,7 +2653,7 @@
       <c r="L122" s="12"/>
     </row>
     <row r="123" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="35"/>
+      <c r="A123" s="36"/>
       <c r="B123" s="5" t="s">
         <v>16</v>
       </c>
@@ -2681,10 +2689,10 @@
       </c>
     </row>
     <row r="126" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="40" t="s">
+      <c r="A126" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B126" s="38"/>
+      <c r="B126" s="39"/>
       <c r="C126" s="19">
         <v>214</v>
       </c>
@@ -2700,16 +2708,16 @@
       <c r="G126" s="19">
         <v>227</v>
       </c>
-      <c r="I126" s="41" t="s">
+      <c r="I126" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J126" s="38"/>
+      <c r="J126" s="39"/>
       <c r="K126" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="127" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="33" t="s">
+      <c r="A127" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B127" s="5" t="s">
@@ -2720,7 +2728,7 @@
       <c r="E127" s="9"/>
       <c r="F127" s="9"/>
       <c r="G127" s="10"/>
-      <c r="I127" s="33" t="s">
+      <c r="I127" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J127" s="5" t="s">
@@ -2729,103 +2737,103 @@
       <c r="K127" s="10"/>
     </row>
     <row r="128" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="34"/>
+      <c r="A128" s="35"/>
       <c r="B128" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G128" s="12"/>
-      <c r="I128" s="34"/>
+      <c r="I128" s="35"/>
       <c r="J128" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K128" s="12"/>
     </row>
     <row r="129" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="34"/>
+      <c r="A129" s="35"/>
       <c r="B129" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G129" s="12"/>
-      <c r="I129" s="34"/>
+      <c r="I129" s="35"/>
       <c r="J129" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K129" s="12"/>
     </row>
     <row r="130" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="34"/>
+      <c r="A130" s="35"/>
       <c r="B130" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G130" s="12"/>
-      <c r="I130" s="34"/>
+      <c r="I130" s="35"/>
       <c r="J130" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K130" s="12"/>
     </row>
     <row r="131" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="34"/>
+      <c r="A131" s="35"/>
       <c r="B131" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G131" s="12"/>
-      <c r="I131" s="34"/>
+      <c r="I131" s="35"/>
       <c r="J131" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K131" s="12"/>
     </row>
     <row r="132" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="34"/>
+      <c r="A132" s="35"/>
       <c r="B132" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G132" s="12"/>
-      <c r="I132" s="34"/>
+      <c r="I132" s="35"/>
       <c r="J132" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K132" s="12"/>
     </row>
     <row r="133" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="34"/>
+      <c r="A133" s="35"/>
       <c r="B133" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G133" s="12"/>
-      <c r="I133" s="34"/>
+      <c r="I133" s="35"/>
       <c r="J133" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K133" s="12"/>
     </row>
     <row r="134" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="34"/>
+      <c r="A134" s="35"/>
       <c r="B134" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G134" s="12"/>
-      <c r="I134" s="34"/>
+      <c r="I134" s="35"/>
       <c r="J134" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K134" s="12"/>
     </row>
     <row r="135" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="34"/>
+      <c r="A135" s="35"/>
       <c r="B135" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G135" s="12"/>
-      <c r="I135" s="34"/>
+      <c r="I135" s="35"/>
       <c r="J135" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K135" s="12"/>
     </row>
     <row r="136" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="35"/>
+      <c r="A136" s="36"/>
       <c r="B136" s="5" t="s">
         <v>16</v>
       </c>
@@ -2844,7 +2852,7 @@
       <c r="G136" s="26">
         <v>1</v>
       </c>
-      <c r="I136" s="35"/>
+      <c r="I136" s="36"/>
       <c r="J136" s="5" t="s">
         <v>16</v>
       </c>
@@ -2864,24 +2872,24 @@
     <row r="140" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="5"/>
       <c r="B140" s="5"/>
-      <c r="C140" s="36" t="s">
+      <c r="C140" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D140" s="37"/>
-      <c r="E140" s="37"/>
-      <c r="F140" s="37"/>
-      <c r="G140" s="37"/>
-      <c r="H140" s="37"/>
-      <c r="I140" s="37"/>
-      <c r="J140" s="37"/>
-      <c r="K140" s="37"/>
-      <c r="L140" s="38"/>
+      <c r="D140" s="38"/>
+      <c r="E140" s="38"/>
+      <c r="F140" s="38"/>
+      <c r="G140" s="38"/>
+      <c r="H140" s="38"/>
+      <c r="I140" s="38"/>
+      <c r="J140" s="38"/>
+      <c r="K140" s="38"/>
+      <c r="L140" s="39"/>
     </row>
     <row r="141" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="39" t="s">
+      <c r="A141" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B141" s="38"/>
+      <c r="B141" s="39"/>
       <c r="C141" s="7" t="s">
         <v>4</v>
       </c>
@@ -2914,7 +2922,7 @@
       </c>
     </row>
     <row r="142" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="33" t="s">
+      <c r="A142" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B142" s="5" t="s">
@@ -2952,7 +2960,7 @@
       </c>
     </row>
     <row r="143" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="34"/>
+      <c r="A143" s="35"/>
       <c r="B143" s="5" t="s">
         <v>8</v>
       </c>
@@ -2960,7 +2968,7 @@
       <c r="L143" s="12"/>
     </row>
     <row r="144" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="34"/>
+      <c r="A144" s="35"/>
       <c r="B144" s="5" t="s">
         <v>9</v>
       </c>
@@ -2968,7 +2976,7 @@
       <c r="L144" s="12"/>
     </row>
     <row r="145" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="34"/>
+      <c r="A145" s="35"/>
       <c r="B145" s="5" t="s">
         <v>10</v>
       </c>
@@ -2976,7 +2984,7 @@
       <c r="L145" s="12"/>
     </row>
     <row r="146" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="34"/>
+      <c r="A146" s="35"/>
       <c r="B146" s="5" t="s">
         <v>11</v>
       </c>
@@ -3012,7 +3020,7 @@
       </c>
     </row>
     <row r="147" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="34"/>
+      <c r="A147" s="35"/>
       <c r="B147" s="5" t="s">
         <v>12</v>
       </c>
@@ -3048,7 +3056,7 @@
       </c>
     </row>
     <row r="148" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="34"/>
+      <c r="A148" s="35"/>
       <c r="B148" s="5" t="s">
         <v>13</v>
       </c>
@@ -3056,7 +3064,7 @@
       <c r="L148" s="12"/>
     </row>
     <row r="149" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="34"/>
+      <c r="A149" s="35"/>
       <c r="B149" s="5" t="s">
         <v>14</v>
       </c>
@@ -3064,7 +3072,7 @@
       <c r="L149" s="12"/>
     </row>
     <row r="150" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="34"/>
+      <c r="A150" s="35"/>
       <c r="B150" s="5" t="s">
         <v>15</v>
       </c>
@@ -3072,7 +3080,7 @@
       <c r="L150" s="12"/>
     </row>
     <row r="151" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="35"/>
+      <c r="A151" s="36"/>
       <c r="B151" s="5" t="s">
         <v>16</v>
       </c>
@@ -3088,10 +3096,10 @@
       <c r="L151" s="17"/>
     </row>
     <row r="154" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="40" t="s">
+      <c r="A154" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B154" s="38"/>
+      <c r="B154" s="39"/>
       <c r="C154" s="19">
         <v>214</v>
       </c>
@@ -3107,16 +3115,16 @@
       <c r="G154" s="19">
         <v>227</v>
       </c>
-      <c r="I154" s="41" t="s">
+      <c r="I154" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J154" s="38"/>
+      <c r="J154" s="39"/>
       <c r="K154" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="33" t="s">
+      <c r="A155" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B155" s="5" t="s">
@@ -3137,7 +3145,7 @@
       <c r="G155" s="32">
         <v>0</v>
       </c>
-      <c r="I155" s="33" t="s">
+      <c r="I155" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J155" s="5" t="s">
@@ -3148,43 +3156,43 @@
       </c>
     </row>
     <row r="156" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="34"/>
+      <c r="A156" s="35"/>
       <c r="B156" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G156" s="12"/>
-      <c r="I156" s="34"/>
+      <c r="I156" s="35"/>
       <c r="J156" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K156" s="12"/>
     </row>
     <row r="157" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="34"/>
+      <c r="A157" s="35"/>
       <c r="B157" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G157" s="12"/>
-      <c r="I157" s="34"/>
+      <c r="I157" s="35"/>
       <c r="J157" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K157" s="12"/>
     </row>
     <row r="158" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="34"/>
+      <c r="A158" s="35"/>
       <c r="B158" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G158" s="12"/>
-      <c r="I158" s="34"/>
+      <c r="I158" s="35"/>
       <c r="J158" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K158" s="12"/>
     </row>
     <row r="159" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="34"/>
+      <c r="A159" s="35"/>
       <c r="B159" s="5" t="s">
         <v>11</v>
       </c>
@@ -3203,7 +3211,7 @@
       <c r="G159" s="27">
         <v>1</v>
       </c>
-      <c r="I159" s="34"/>
+      <c r="I159" s="35"/>
       <c r="J159" s="5" t="s">
         <v>11</v>
       </c>
@@ -3212,7 +3220,7 @@
       </c>
     </row>
     <row r="160" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="34"/>
+      <c r="A160" s="35"/>
       <c r="B160" s="5" t="s">
         <v>12</v>
       </c>
@@ -3231,7 +3239,7 @@
       <c r="G160" s="27">
         <v>1</v>
       </c>
-      <c r="I160" s="34"/>
+      <c r="I160" s="35"/>
       <c r="J160" s="5" t="s">
         <v>12</v>
       </c>
@@ -3240,43 +3248,43 @@
       </c>
     </row>
     <row r="161" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="34"/>
+      <c r="A161" s="35"/>
       <c r="B161" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G161" s="12"/>
-      <c r="I161" s="34"/>
+      <c r="I161" s="35"/>
       <c r="J161" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K161" s="12"/>
     </row>
     <row r="162" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="34"/>
+      <c r="A162" s="35"/>
       <c r="B162" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G162" s="12"/>
-      <c r="I162" s="34"/>
+      <c r="I162" s="35"/>
       <c r="J162" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K162" s="12"/>
     </row>
     <row r="163" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="34"/>
+      <c r="A163" s="35"/>
       <c r="B163" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G163" s="12"/>
-      <c r="I163" s="34"/>
+      <c r="I163" s="35"/>
       <c r="J163" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K163" s="12"/>
     </row>
     <row r="164" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="35"/>
+      <c r="A164" s="36"/>
       <c r="B164" s="5" t="s">
         <v>16</v>
       </c>
@@ -3285,7 +3293,7 @@
       <c r="E164" s="15"/>
       <c r="F164" s="15"/>
       <c r="G164" s="17"/>
-      <c r="I164" s="35"/>
+      <c r="I164" s="36"/>
       <c r="J164" s="5" t="s">
         <v>16</v>
       </c>
@@ -3299,31 +3307,31 @@
       <c r="C167" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D167" s="44" t="s">
+      <c r="D167" s="33" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="5"/>
       <c r="B168" s="5"/>
-      <c r="C168" s="36" t="s">
+      <c r="C168" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D168" s="37"/>
-      <c r="E168" s="37"/>
-      <c r="F168" s="37"/>
-      <c r="G168" s="37"/>
-      <c r="H168" s="37"/>
-      <c r="I168" s="37"/>
-      <c r="J168" s="37"/>
-      <c r="K168" s="37"/>
-      <c r="L168" s="38"/>
+      <c r="D168" s="38"/>
+      <c r="E168" s="38"/>
+      <c r="F168" s="38"/>
+      <c r="G168" s="38"/>
+      <c r="H168" s="38"/>
+      <c r="I168" s="38"/>
+      <c r="J168" s="38"/>
+      <c r="K168" s="38"/>
+      <c r="L168" s="39"/>
     </row>
     <row r="169" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="39" t="s">
+      <c r="A169" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B169" s="38"/>
+      <c r="B169" s="39"/>
       <c r="C169" s="7" t="s">
         <v>4</v>
       </c>
@@ -3356,7 +3364,7 @@
       </c>
     </row>
     <row r="170" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="33" t="s">
+      <c r="A170" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B170" s="5" t="s">
@@ -3394,7 +3402,7 @@
       </c>
     </row>
     <row r="171" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="34"/>
+      <c r="A171" s="35"/>
       <c r="B171" s="5" t="s">
         <v>8</v>
       </c>
@@ -3402,7 +3410,7 @@
       <c r="L171" s="12"/>
     </row>
     <row r="172" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="34"/>
+      <c r="A172" s="35"/>
       <c r="B172" s="5" t="s">
         <v>9</v>
       </c>
@@ -3410,7 +3418,7 @@
       <c r="L172" s="12"/>
     </row>
     <row r="173" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="34"/>
+      <c r="A173" s="35"/>
       <c r="B173" s="5" t="s">
         <v>10</v>
       </c>
@@ -3418,7 +3426,7 @@
       <c r="L173" s="12"/>
     </row>
     <row r="174" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="34"/>
+      <c r="A174" s="35"/>
       <c r="B174" s="5" t="s">
         <v>11</v>
       </c>
@@ -3454,7 +3462,7 @@
       </c>
     </row>
     <row r="175" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="34"/>
+      <c r="A175" s="35"/>
       <c r="B175" s="5" t="s">
         <v>12</v>
       </c>
@@ -3490,7 +3498,7 @@
       </c>
     </row>
     <row r="176" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="34"/>
+      <c r="A176" s="35"/>
       <c r="B176" s="5" t="s">
         <v>13</v>
       </c>
@@ -3498,7 +3506,7 @@
       <c r="L176" s="12"/>
     </row>
     <row r="177" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="34"/>
+      <c r="A177" s="35"/>
       <c r="B177" s="5" t="s">
         <v>14</v>
       </c>
@@ -3506,7 +3514,7 @@
       <c r="L177" s="12"/>
     </row>
     <row r="178" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="34"/>
+      <c r="A178" s="35"/>
       <c r="B178" s="5" t="s">
         <v>15</v>
       </c>
@@ -3514,11 +3522,14 @@
       <c r="L178" s="12"/>
     </row>
     <row r="179" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="35"/>
+      <c r="A179" s="36"/>
       <c r="B179" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C179" s="13"/>
+      <c r="C179" s="13">
+        <f>AVERAGE(C123,C39,C13)</f>
+        <v>43622.666666666664</v>
+      </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15"/>
       <c r="F179" s="15"/>
@@ -3530,10 +3541,10 @@
       <c r="L179" s="17"/>
     </row>
     <row r="182" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="40" t="s">
+      <c r="A182" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B182" s="38"/>
+      <c r="B182" s="39"/>
       <c r="C182" s="19">
         <v>214</v>
       </c>
@@ -3549,16 +3560,16 @@
       <c r="G182" s="19">
         <v>227</v>
       </c>
-      <c r="I182" s="41" t="s">
+      <c r="I182" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J182" s="38"/>
+      <c r="J182" s="39"/>
       <c r="K182" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="33" t="s">
+      <c r="A183" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B183" s="5" t="s">
@@ -3579,7 +3590,7 @@
       <c r="G183" s="32">
         <v>0</v>
       </c>
-      <c r="I183" s="33" t="s">
+      <c r="I183" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J183" s="5" t="s">
@@ -3590,43 +3601,43 @@
       </c>
     </row>
     <row r="184" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="34"/>
+      <c r="A184" s="35"/>
       <c r="B184" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G184" s="12"/>
-      <c r="I184" s="34"/>
+      <c r="I184" s="35"/>
       <c r="J184" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K184" s="12"/>
     </row>
     <row r="185" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="34"/>
+      <c r="A185" s="35"/>
       <c r="B185" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G185" s="12"/>
-      <c r="I185" s="34"/>
+      <c r="I185" s="35"/>
       <c r="J185" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K185" s="12"/>
     </row>
     <row r="186" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="34"/>
+      <c r="A186" s="35"/>
       <c r="B186" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G186" s="12"/>
-      <c r="I186" s="34"/>
+      <c r="I186" s="35"/>
       <c r="J186" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K186" s="12"/>
     </row>
     <row r="187" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="34"/>
+      <c r="A187" s="35"/>
       <c r="B187" s="5" t="s">
         <v>11</v>
       </c>
@@ -3645,7 +3656,7 @@
       <c r="G187" s="27">
         <v>1</v>
       </c>
-      <c r="I187" s="34"/>
+      <c r="I187" s="35"/>
       <c r="J187" s="5" t="s">
         <v>11</v>
       </c>
@@ -3654,7 +3665,7 @@
       </c>
     </row>
     <row r="188" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="34"/>
+      <c r="A188" s="35"/>
       <c r="B188" s="5" t="s">
         <v>12</v>
       </c>
@@ -3673,7 +3684,7 @@
       <c r="G188" s="27">
         <v>1</v>
       </c>
-      <c r="I188" s="34"/>
+      <c r="I188" s="35"/>
       <c r="J188" s="5" t="s">
         <v>12</v>
       </c>
@@ -3682,52 +3693,67 @@
       </c>
     </row>
     <row r="189" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="34"/>
+      <c r="A189" s="35"/>
       <c r="B189" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G189" s="12"/>
-      <c r="I189" s="34"/>
+      <c r="I189" s="35"/>
       <c r="J189" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K189" s="12"/>
     </row>
     <row r="190" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="34"/>
+      <c r="A190" s="35"/>
       <c r="B190" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G190" s="12"/>
-      <c r="I190" s="34"/>
+      <c r="I190" s="35"/>
       <c r="J190" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K190" s="12"/>
     </row>
     <row r="191" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="34"/>
+      <c r="A191" s="35"/>
       <c r="B191" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G191" s="12"/>
-      <c r="I191" s="34"/>
+      <c r="I191" s="35"/>
       <c r="J191" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K191" s="12"/>
     </row>
     <row r="192" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="35"/>
+      <c r="A192" s="36"/>
       <c r="B192" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C192" s="15"/>
-      <c r="D192" s="15"/>
-      <c r="E192" s="15"/>
-      <c r="F192" s="15"/>
-      <c r="G192" s="17"/>
-      <c r="I192" s="35"/>
+      <c r="C192" s="15">
+        <f>AVERAGE(C136,C52,C26)</f>
+        <v>1</v>
+      </c>
+      <c r="D192" s="15">
+        <f>AVERAGE(D136,D52,D26)</f>
+        <v>1</v>
+      </c>
+      <c r="E192" s="15">
+        <f>AVERAGE(E136,E52,E26)</f>
+        <v>1</v>
+      </c>
+      <c r="F192" s="15">
+        <f>AVERAGE(F136,F52,F26)</f>
+        <v>1</v>
+      </c>
+      <c r="G192" s="17">
+        <f>AVERAGE(G136,G52,G26)</f>
+        <v>1</v>
+      </c>
+      <c r="I192" s="36"/>
       <c r="J192" s="5" t="s">
         <v>16</v>
       </c>
@@ -3735,6 +3761,46 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="I17:I26"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:A39"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="I43:I52"/>
+    <mergeCell ref="C41:L41"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:A67"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="A71:A80"/>
+    <mergeCell ref="I71:I80"/>
+    <mergeCell ref="C84:L84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:A95"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="A99:A108"/>
+    <mergeCell ref="I99:I108"/>
+    <mergeCell ref="C112:L112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:A123"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="I126:J126"/>
+    <mergeCell ref="A127:A136"/>
+    <mergeCell ref="I127:I136"/>
+    <mergeCell ref="C140:L140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A142:A151"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="I154:J154"/>
     <mergeCell ref="A182:B182"/>
     <mergeCell ref="I182:J182"/>
     <mergeCell ref="A183:A192"/>
@@ -3744,46 +3810,6 @@
     <mergeCell ref="C168:L168"/>
     <mergeCell ref="A169:B169"/>
     <mergeCell ref="A170:A179"/>
-    <mergeCell ref="C140:L140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A142:A151"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="I154:J154"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:A123"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="I126:J126"/>
-    <mergeCell ref="A127:A136"/>
-    <mergeCell ref="I127:I136"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="I98:J98"/>
-    <mergeCell ref="A99:A108"/>
-    <mergeCell ref="I99:I108"/>
-    <mergeCell ref="C112:L112"/>
-    <mergeCell ref="A71:A80"/>
-    <mergeCell ref="I71:I80"/>
-    <mergeCell ref="C84:L84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:A95"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:A67"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:A39"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="A43:A52"/>
-    <mergeCell ref="I43:I52"/>
-    <mergeCell ref="C41:L41"/>
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I17:I26"/>
-    <mergeCell ref="I16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3849,18 +3875,18 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -3868,10 +3894,10 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -3904,7 +3930,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3922,7 +3948,7 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -3930,7 +3956,7 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -3938,7 +3964,7 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -3946,7 +3972,7 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
@@ -3954,7 +3980,7 @@
       <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -3962,7 +3988,7 @@
       <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -3970,7 +3996,7 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -3978,7 +4004,7 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -3986,7 +4012,7 @@
       <c r="L12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -4022,10 +4048,10 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="19">
         <v>214</v>
       </c>
@@ -4041,16 +4067,16 @@
       <c r="G16" s="19">
         <v>227</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -4061,7 +4087,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="10"/>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -4070,103 +4096,103 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="I18" s="34"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="I20" s="34"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="I21" s="34"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="I22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="12"/>
-      <c r="I23" s="34"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="I24" s="34"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="I25" s="34"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -4185,7 +4211,7 @@
       <c r="G26" s="26">
         <v>1</v>
       </c>
-      <c r="I26" s="35"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="5" t="s">
         <v>16</v>
       </c>
@@ -4237,18 +4263,18 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -4256,10 +4282,10 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -4292,7 +4318,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -4310,7 +4336,7 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -4318,7 +4344,7 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -4326,7 +4352,7 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -4334,7 +4360,7 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
@@ -4342,7 +4368,7 @@
       <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -4350,7 +4376,7 @@
       <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -4358,7 +4384,7 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -4366,7 +4392,7 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -4402,7 +4428,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -4418,10 +4444,10 @@
       <c r="L13" s="17"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="19">
         <v>214</v>
       </c>
@@ -4437,16 +4463,16 @@
       <c r="G16" s="19">
         <v>227</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -4457,7 +4483,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="10"/>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -4466,91 +4492,91 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="I18" s="34"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="I20" s="34"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="I21" s="34"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="I22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="12"/>
-      <c r="I23" s="34"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="I24" s="34"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
@@ -4569,7 +4595,7 @@
       <c r="G25" s="27">
         <v>1</v>
       </c>
-      <c r="I25" s="34"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="5" t="s">
         <v>15</v>
       </c>
@@ -4578,7 +4604,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -4587,7 +4613,7 @@
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="17"/>
-      <c r="I26" s="35"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="5" t="s">
         <v>16</v>
       </c>
@@ -4639,18 +4665,18 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -4658,10 +4684,10 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -4694,7 +4720,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -4712,7 +4738,7 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -4720,7 +4746,7 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -4728,7 +4754,7 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -4736,7 +4762,7 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
@@ -4744,7 +4770,7 @@
       <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -4752,7 +4778,7 @@
       <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -4788,7 +4814,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -4824,7 +4850,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -4832,7 +4858,7 @@
       <c r="L12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -4848,10 +4874,10 @@
       <c r="L13" s="17"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="19">
         <v>214</v>
       </c>
@@ -4867,16 +4893,16 @@
       <c r="G16" s="19">
         <v>227</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -4887,7 +4913,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="10"/>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -4896,67 +4922,67 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="I18" s="34"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="I20" s="34"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="I21" s="34"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="I22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
@@ -4975,7 +5001,7 @@
       <c r="G23" s="27">
         <v>1</v>
       </c>
-      <c r="I23" s="34"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
@@ -4984,7 +5010,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
@@ -5003,7 +5029,7 @@
       <c r="G24" s="27">
         <v>1</v>
       </c>
-      <c r="I24" s="34"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="5" t="s">
         <v>14</v>
       </c>
@@ -5012,19 +5038,19 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="I25" s="34"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -5033,7 +5059,7 @@
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="17"/>
-      <c r="I26" s="35"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="5" t="s">
         <v>16</v>
       </c>
@@ -5083,18 +5109,18 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -5102,10 +5128,10 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -5138,7 +5164,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -5156,7 +5182,7 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -5164,7 +5190,7 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -5172,7 +5198,7 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -5180,7 +5206,7 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
@@ -5188,7 +5214,7 @@
       <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -5196,7 +5222,7 @@
       <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -5204,7 +5230,7 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -5212,7 +5238,7 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -5220,7 +5246,7 @@
       <c r="L12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -5256,10 +5282,10 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="19">
         <v>214</v>
       </c>
@@ -5275,16 +5301,16 @@
       <c r="G16" s="19">
         <v>227</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -5295,7 +5321,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="10"/>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -5304,103 +5330,103 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="I18" s="34"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="I20" s="34"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="I21" s="34"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="12"/>
-      <c r="I22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="12"/>
-      <c r="I23" s="34"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="I24" s="34"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="I25" s="34"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -5419,7 +5445,7 @@
       <c r="G26" s="26">
         <v>1</v>
       </c>
-      <c r="I26" s="35"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="5" t="s">
         <v>16</v>
       </c>
@@ -5471,18 +5497,18 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -5490,10 +5516,10 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
@@ -5526,7 +5552,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -5564,7 +5590,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -5572,7 +5598,7 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -5580,7 +5606,7 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -5588,7 +5614,7 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
@@ -5624,7 +5650,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -5660,7 +5686,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -5668,7 +5694,7 @@
       <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -5676,7 +5702,7 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -5684,7 +5710,7 @@
       <c r="L12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -5700,10 +5726,10 @@
       <c r="L13" s="17"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="19">
         <v>214</v>
       </c>
@@ -5719,16 +5745,16 @@
       <c r="G16" s="19">
         <v>227</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="20">
         <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -5749,7 +5775,7 @@
       <c r="G17" s="32">
         <v>0</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="5" t="s">
@@ -5760,43 +5786,43 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="12"/>
-      <c r="I18" s="34"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="12"/>
-      <c r="I19" s="34"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="12"/>
-      <c r="I20" s="34"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
@@ -5815,7 +5841,7 @@
       <c r="G21" s="27">
         <v>1</v>
       </c>
-      <c r="I21" s="34"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="5" t="s">
         <v>11</v>
       </c>
@@ -5824,7 +5850,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
@@ -5843,7 +5869,7 @@
       <c r="G22" s="27">
         <v>1</v>
       </c>
-      <c r="I22" s="34"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="5" t="s">
         <v>12</v>
       </c>
@@ -5852,43 +5878,43 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="12"/>
-      <c r="I23" s="34"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="I24" s="34"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="12"/>
-      <c r="I25" s="34"/>
+      <c r="I25" s="35"/>
       <c r="J25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -5897,7 +5923,7 @@
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="17"/>
-      <c r="I26" s="35"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="5" t="s">
         <v>16</v>
       </c>

</xml_diff>